<commit_message>
remove a picture of table inside the excel
</commit_message>
<xml_diff>
--- a/run_information.xlsx
+++ b/run_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunhalee/Documents/LOCAETA/LOCAETA_AQ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983E5805-0D42-E545-ACCB-BE0BEE2E9BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D464A45D-3DE8-D44D-8F48-55E8EA0252E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3680" yWindow="500" windowWidth="26640" windowHeight="18740" xr2:uid="{193FCF14-7D99-9742-A76C-A64B96D7F43A}"/>
+    <workbookView xWindow="12080" yWindow="500" windowWidth="26640" windowHeight="18740" xr2:uid="{193FCF14-7D99-9742-A76C-A64B96D7F43A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,9 +107,6 @@
     <t>2050_easyhard_decarb95_Food_Agr</t>
   </si>
   <si>
-    <t>Full_USA scenario</t>
-  </si>
-  <si>
     <t>Food and Agriculture sectors only</t>
   </si>
   <si>
@@ -149,6 +146,9 @@
   <si>
     <t>each run has its own base emissions
 : run name + "_base"</t>
+  </si>
+  <si>
+    <t>Full USA scenario</t>
   </si>
 </sst>
 </file>
@@ -647,7 +647,7 @@
   <dimension ref="B1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -668,10 +668,10 @@
         <v>11</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>18</v>
@@ -685,13 +685,13 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="23" customHeight="1" x14ac:dyDescent="0.2">
@@ -718,7 +718,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -738,7 +738,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -760,10 +760,10 @@
         <v>3</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>19</v>
@@ -795,13 +795,13 @@
         <v>7</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -828,7 +828,7 @@
         <v>20</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>

</xml_diff>